<commit_message>
Regenerate sample Excel file with exactly 100 records
</commit_message>
<xml_diff>
--- a/public/sample-attendance.xlsx
+++ b/public/sample-attendance.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="7">
   <si>
     <t>Employee Name</t>
   </si>
@@ -28,10 +28,10 @@
     <t>Sarah Johnson</t>
   </si>
   <si>
-    <t>John Smith</t>
+    <t/>
   </si>
   <si>
-    <t/>
+    <t>John Smith</t>
   </si>
 </sst>
 </file>
@@ -455,10 +455,10 @@
         <v>45291.77083333333</v>
       </c>
       <c r="C2" s="2">
-        <v>45292.209027777775</v>
+        <v>45292.21388888889</v>
       </c>
       <c r="D2" s="2">
-        <v>45292.53402777778</v>
+        <v>45292.521527777775</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -469,10 +469,10 @@
         <v>45292.77083333333</v>
       </c>
       <c r="C3" s="2">
-        <v>45293.20694444445</v>
+        <v>45293.20833333333</v>
       </c>
       <c r="D3" s="2">
-        <v>45293.52847222222</v>
+        <v>45293.55</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -483,10 +483,10 @@
         <v>45293.77083333333</v>
       </c>
       <c r="C4" s="2">
-        <v>45294.21805555555</v>
+        <v>45294.209027777775</v>
       </c>
       <c r="D4" s="2">
-        <v>45294.544444444444</v>
+        <v>45294.52916666667</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,10 +497,10 @@
         <v>45294.77083333333</v>
       </c>
       <c r="C5" s="2">
-        <v>45295.21736111111</v>
+        <v>45295.19583333333</v>
       </c>
       <c r="D5" s="2">
-        <v>45295.53263888889</v>
+        <v>45295.523611111115</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -511,10 +511,10 @@
         <v>45295.77083333333</v>
       </c>
       <c r="C6" s="2">
-        <v>45296.21319444444</v>
+        <v>45296.214583333334</v>
       </c>
       <c r="D6" s="2">
-        <v>45296.54652777778</v>
+        <v>45296.53611111111</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,11 +524,11 @@
       <c r="B7" s="1">
         <v>45296.77083333333</v>
       </c>
-      <c r="C7" s="2">
-        <v>45297.1875</v>
-      </c>
-      <c r="D7" s="2">
-        <v>45297.35416666667</v>
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -539,10 +539,10 @@
         <v>45298.77083333333</v>
       </c>
       <c r="C8" s="2">
-        <v>45299.19652777778</v>
+        <v>45299.195138888885</v>
       </c>
       <c r="D8" s="2">
-        <v>45299.53472222222</v>
+        <v>45299.544444444444</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -553,10 +553,10 @@
         <v>45299.77083333333</v>
       </c>
       <c r="C9" s="2">
-        <v>45300.205555555556</v>
+        <v>45300.197222222225</v>
       </c>
       <c r="D9" s="2">
-        <v>45300.53611111111</v>
+        <v>45300.54583333334</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -567,29 +567,29 @@
         <v>45300.77083333333</v>
       </c>
       <c r="C10" s="2">
-        <v>45301.20763888889</v>
+        <v>45301.195138888885</v>
       </c>
       <c r="D10" s="2">
-        <v>45301.5375</v>
+        <v>45301.53333333333</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1">
         <v>45322.77083333333</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
+      <c r="C11" s="2">
+        <v>45323.18888888889</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45323.53055555555</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1">
         <v>45323.77083333333</v>
@@ -598,96 +598,96 @@
         <v>45324.21388888889</v>
       </c>
       <c r="D12" s="2">
-        <v>45324.53958333333</v>
+        <v>45324.52291666667</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1">
         <v>45324.77083333333</v>
       </c>
-      <c r="C13" s="2">
-        <v>45325.1875</v>
-      </c>
-      <c r="D13" s="2">
-        <v>45325.35416666667</v>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1">
         <v>45326.77083333333</v>
       </c>
       <c r="C14" s="2">
-        <v>45327.19930555555</v>
+        <v>45327.21041666667</v>
       </c>
       <c r="D14" s="2">
-        <v>45327.53958333333</v>
+        <v>45327.54513888889</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1">
         <v>45327.77083333333</v>
       </c>
       <c r="C15" s="2">
-        <v>45328.20694444445</v>
+        <v>45328.19652777778</v>
       </c>
       <c r="D15" s="2">
-        <v>45328.525</v>
+        <v>45328.53680555556</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1">
         <v>45328.77083333333</v>
       </c>
       <c r="C16" s="2">
-        <v>45329.205555555556</v>
+        <v>45329.19861111111</v>
       </c>
       <c r="D16" s="2">
-        <v>45329.54791666666</v>
+        <v>45329.523611111115</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <v>45329.77083333333</v>
       </c>
       <c r="C17" s="2">
-        <v>45330.194444444445</v>
+        <v>45330.20138888889</v>
       </c>
       <c r="D17" s="2">
-        <v>45330.53680555556</v>
+        <v>45330.52916666667</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1">
         <v>45330.77083333333</v>
       </c>
       <c r="C18" s="2">
-        <v>45331.194444444445</v>
+        <v>45331.20277777778</v>
       </c>
       <c r="D18" s="2">
-        <v>45331.54861111111</v>
+        <v>45331.54375</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1">
         <v>45331.77083333333</v>
@@ -707,10 +707,10 @@
         <v>45351.77083333333</v>
       </c>
       <c r="C20" s="2">
-        <v>45352.18888888889</v>
+        <v>45352.21388888889</v>
       </c>
       <c r="D20" s="2">
-        <v>45352.50833333333</v>
+        <v>45352.575694444444</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -720,11 +720,11 @@
       <c r="B21" s="1">
         <v>45352.77083333333</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>6</v>
+      <c r="C21" s="2">
+        <v>45353.1875</v>
+      </c>
+      <c r="D21" s="2">
+        <v>45353.35416666667</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,10 +735,10 @@
         <v>45354.77083333333</v>
       </c>
       <c r="C22" s="2">
-        <v>45355.19236111111</v>
+        <v>45355.191666666666</v>
       </c>
       <c r="D22" s="2">
-        <v>45355.53333333333</v>
+        <v>45355.54305555555</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,10 +749,10 @@
         <v>45355.77083333333</v>
       </c>
       <c r="C23" s="2">
-        <v>45356.20208333334</v>
+        <v>45356.19791666667</v>
       </c>
       <c r="D23" s="2">
-        <v>45356.54236111111</v>
+        <v>45356.527083333334</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -762,11 +762,11 @@
       <c r="B24" s="1">
         <v>45356.77083333333</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>6</v>
+      <c r="C24" s="2">
+        <v>45357.2125</v>
+      </c>
+      <c r="D24" s="2">
+        <v>45357.52222222222</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,10 +777,10 @@
         <v>45357.77083333333</v>
       </c>
       <c r="C25" s="2">
-        <v>45358.20486111111</v>
+        <v>45358.19375</v>
       </c>
       <c r="D25" s="2">
-        <v>45358.538194444445</v>
+        <v>45358.540972222225</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,10 +791,10 @@
         <v>45358.77083333333</v>
       </c>
       <c r="C26" s="2">
-        <v>45359.20277777778</v>
+        <v>45359.19791666667</v>
       </c>
       <c r="D26" s="2">
-        <v>45359.54791666666</v>
+        <v>45359.549305555556</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,85 +819,85 @@
         <v>45361.77083333333</v>
       </c>
       <c r="C28" s="2">
-        <v>45362.20208333334</v>
+        <v>45362.20833333333</v>
       </c>
       <c r="D28" s="2">
-        <v>45362.53194444445</v>
+        <v>45362.53333333333</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1">
         <v>45382.77083333333</v>
       </c>
       <c r="C29" s="2">
-        <v>45383.20763888889</v>
+        <v>45383.18888888889</v>
       </c>
       <c r="D29" s="2">
-        <v>45383.53611111111</v>
+        <v>45383.544444444444</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1">
         <v>45383.77083333333</v>
       </c>
       <c r="C30" s="2">
-        <v>45384.19791666667</v>
+        <v>45384.18819444445</v>
       </c>
       <c r="D30" s="2">
-        <v>45384.540972222225</v>
+        <v>45384.53680555556</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1">
         <v>45384.77083333333</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>6</v>
+      <c r="C31" s="2">
+        <v>45385.18888888889</v>
+      </c>
+      <c r="D31" s="2">
+        <v>45385.53611111111</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1">
         <v>45385.77083333333</v>
       </c>
-      <c r="C32" s="2">
-        <v>45386.19236111111</v>
-      </c>
-      <c r="D32" s="2">
-        <v>45386.52638888889</v>
+      <c r="C32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1">
         <v>45386.77083333333</v>
       </c>
       <c r="C33" s="2">
-        <v>45387.20833333333</v>
+        <v>45387.20763888889</v>
       </c>
       <c r="D33" s="2">
-        <v>45387.53611111111</v>
+        <v>45387.54027777778</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1">
         <v>45387.77083333333</v>
@@ -911,44 +911,44 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1">
         <v>45389.77083333333</v>
       </c>
       <c r="C35" s="2">
-        <v>45390.205555555556</v>
+        <v>45390.20833333333</v>
       </c>
       <c r="D35" s="2">
-        <v>45390.53194444445</v>
+        <v>45390.52847222222</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36" s="1">
         <v>45390.77083333333</v>
       </c>
       <c r="C36" s="2">
-        <v>45391.21388888889</v>
+        <v>45391.19861111111</v>
       </c>
       <c r="D36" s="2">
-        <v>45391.57777777778</v>
+        <v>45391.54791666666</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1">
         <v>45391.77083333333</v>
       </c>
       <c r="C37" s="2">
-        <v>45392.19305555556</v>
+        <v>45392.21319444444</v>
       </c>
       <c r="D37" s="2">
-        <v>45392.52986111111</v>
+        <v>45392.549305555556</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -959,10 +959,10 @@
         <v>45412.77083333333</v>
       </c>
       <c r="C38" s="2">
-        <v>45413.19861111111</v>
+        <v>45413.214583333334</v>
       </c>
       <c r="D38" s="2">
-        <v>45413.5375</v>
+        <v>45413.570138888885</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -973,10 +973,10 @@
         <v>45413.77083333333</v>
       </c>
       <c r="C39" s="2">
-        <v>45414.18888888889</v>
+        <v>45414.19583333333</v>
       </c>
       <c r="D39" s="2">
-        <v>45414.53680555556</v>
+        <v>45414.53472222222</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -987,10 +987,10 @@
         <v>45414.77083333333</v>
       </c>
       <c r="C40" s="2">
-        <v>45415.214583333334</v>
+        <v>45415.20347222222</v>
       </c>
       <c r="D40" s="2">
-        <v>45415.544444444444</v>
+        <v>45415.53472222222</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1000,11 +1000,11 @@
       <c r="B41" s="1">
         <v>45415.77083333333</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>6</v>
+      <c r="C41" s="2">
+        <v>45416.1875</v>
+      </c>
+      <c r="D41" s="2">
+        <v>45416.35416666667</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1015,10 +1015,10 @@
         <v>45417.77083333333</v>
       </c>
       <c r="C42" s="2">
-        <v>45418.20277777778</v>
+        <v>45418.20486111111</v>
       </c>
       <c r="D42" s="2">
-        <v>45418.54791666666</v>
+        <v>45418.55069444445</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1029,10 +1029,10 @@
         <v>45418.77083333333</v>
       </c>
       <c r="C43" s="2">
-        <v>45419.21388888889</v>
+        <v>45419.20138888889</v>
       </c>
       <c r="D43" s="2">
-        <v>45419.53125</v>
+        <v>45419.52013888889</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1043,10 +1043,10 @@
         <v>45419.77083333333</v>
       </c>
       <c r="C44" s="2">
-        <v>45420.19027777778</v>
+        <v>45420.21041666667</v>
       </c>
       <c r="D44" s="2">
-        <v>45420.52916666667</v>
+        <v>45420.52986111111</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,113 +1057,113 @@
         <v>45420.77083333333</v>
       </c>
       <c r="C45" s="2">
-        <v>45421.21597222222</v>
+        <v>45421.214583333334</v>
       </c>
       <c r="D45" s="2">
-        <v>45421.54722222222</v>
+        <v>45421.53055555555</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1">
         <v>45443.77083333333</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1">
         <v>45445.77083333333</v>
       </c>
       <c r="C47" s="2">
-        <v>45446.20208333334</v>
+        <v>45446.21319444444</v>
       </c>
       <c r="D47" s="2">
-        <v>45446.527083333334</v>
+        <v>45446.525</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1">
         <v>45446.77083333333</v>
       </c>
       <c r="C48" s="2">
-        <v>45447.2125</v>
+        <v>45447.19027777778</v>
       </c>
       <c r="D48" s="2">
-        <v>45447.523611111115</v>
+        <v>45447.527083333334</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1">
         <v>45447.77083333333</v>
       </c>
       <c r="C49" s="2">
-        <v>45448.21041666667</v>
+        <v>45448.209027777775</v>
       </c>
       <c r="D49" s="2">
-        <v>45448.53611111111</v>
+        <v>45448.53680555556</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1">
         <v>45448.77083333333</v>
       </c>
       <c r="C50" s="2">
-        <v>45449.211805555555</v>
+        <v>45449.2125</v>
       </c>
       <c r="D50" s="2">
-        <v>45449.52916666667</v>
+        <v>45449.53402777778</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1">
         <v>45449.77083333333</v>
       </c>
       <c r="C51" s="2">
-        <v>45450.19791666667</v>
+        <v>45450.211111111115</v>
       </c>
       <c r="D51" s="2">
-        <v>45450.57777777778</v>
+        <v>45450.54583333334</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1">
         <v>45450.77083333333</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B53" s="1">
         <v>45452.77083333333</v>
@@ -1172,7 +1172,7 @@
         <v>45453.21805555555</v>
       </c>
       <c r="D53" s="2">
-        <v>45453.53402777778</v>
+        <v>45453.55138888889</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1183,10 +1183,10 @@
         <v>45473.77083333333</v>
       </c>
       <c r="C54" s="2">
-        <v>45474.197222222225</v>
+        <v>45474.18819444445</v>
       </c>
       <c r="D54" s="2">
-        <v>45474.52569444444</v>
+        <v>45474.54722222222</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,10 +1197,10 @@
         <v>45474.77083333333</v>
       </c>
       <c r="C55" s="2">
-        <v>45475.20277777778</v>
+        <v>45475.21319444444</v>
       </c>
       <c r="D55" s="2">
-        <v>45475.538888888885</v>
+        <v>45475.52638888889</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,11 +1210,11 @@
       <c r="B56" s="1">
         <v>45475.77083333333</v>
       </c>
-      <c r="C56" s="2">
-        <v>45476.19652777778</v>
-      </c>
-      <c r="D56" s="2">
-        <v>45476.54583333334</v>
+      <c r="C56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1225,10 +1225,10 @@
         <v>45476.77083333333</v>
       </c>
       <c r="C57" s="2">
-        <v>45477.205555555556</v>
+        <v>45477.21319444444</v>
       </c>
       <c r="D57" s="2">
-        <v>45477.540972222225</v>
+        <v>45477.524305555555</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,10 +1239,10 @@
         <v>45477.77083333333</v>
       </c>
       <c r="C58" s="2">
-        <v>45478.21666666667</v>
+        <v>45478.211111111115</v>
       </c>
       <c r="D58" s="2">
-        <v>45478.54027777778</v>
+        <v>45478.55069444445</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,11 +1252,11 @@
       <c r="B59" s="1">
         <v>45478.77083333333</v>
       </c>
-      <c r="C59" s="2">
-        <v>45479.1875</v>
-      </c>
-      <c r="D59" s="2">
-        <v>45479.35416666667</v>
+      <c r="C59" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,10 +1267,10 @@
         <v>45480.77083333333</v>
       </c>
       <c r="C60" s="2">
-        <v>45481.205555555556</v>
+        <v>45481.2</v>
       </c>
       <c r="D60" s="2">
-        <v>45481.53333333333</v>
+        <v>45481.544444444444</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1281,43 +1281,43 @@
         <v>45481.77083333333</v>
       </c>
       <c r="C61" s="2">
-        <v>45482.209027777775</v>
+        <v>45482.21597222222</v>
       </c>
       <c r="D61" s="2">
-        <v>45482.53402777778</v>
+        <v>45482.52569444444</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B62" s="1">
         <v>45504.77083333333</v>
       </c>
       <c r="C62" s="2">
-        <v>45505.18888888889</v>
+        <v>45505.2</v>
       </c>
       <c r="D62" s="2">
-        <v>45505.524305555555</v>
+        <v>45505.538888888885</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B63" s="1">
         <v>45505.77083333333</v>
       </c>
       <c r="C63" s="2">
-        <v>45506.21388888889</v>
+        <v>45506.20138888889</v>
       </c>
       <c r="D63" s="2">
-        <v>45506.53958333333</v>
+        <v>45506.521527777775</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B64" s="1">
         <v>45506.77083333333</v>
@@ -1331,72 +1331,72 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B65" s="1">
         <v>45508.77083333333</v>
       </c>
       <c r="C65" s="2">
-        <v>45509.20694444445</v>
+        <v>45509.2</v>
       </c>
       <c r="D65" s="2">
-        <v>45509.53611111111</v>
+        <v>45509.5375</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1">
         <v>45509.77083333333</v>
       </c>
       <c r="C66" s="2">
-        <v>45510.20416666666</v>
+        <v>45510.21388888889</v>
       </c>
       <c r="D66" s="2">
-        <v>45510.54861111111</v>
+        <v>45510.54027777778</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B67" s="1">
         <v>45510.77083333333</v>
       </c>
       <c r="C67" s="2">
-        <v>45511.194444444445</v>
+        <v>45511.21388888889</v>
       </c>
       <c r="D67" s="2">
-        <v>45511.538194444445</v>
+        <v>45511.53402777778</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B68" s="1">
         <v>45511.77083333333</v>
       </c>
       <c r="C68" s="2">
-        <v>45512.18958333333</v>
+        <v>45512.20694444445</v>
       </c>
       <c r="D68" s="2">
-        <v>45512.5375</v>
+        <v>45512.53263888889</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B69" s="1">
         <v>45512.77083333333</v>
       </c>
-      <c r="C69" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>6</v>
+      <c r="C69" s="2">
+        <v>45513.19027777778</v>
+      </c>
+      <c r="D69" s="2">
+        <v>45513.538194444445</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1407,10 +1407,10 @@
         <v>45536.77083333333</v>
       </c>
       <c r="C70" s="2">
-        <v>45537.211111111115</v>
+        <v>45537.19930555555</v>
       </c>
       <c r="D70" s="2">
-        <v>45537.540972222225</v>
+        <v>45537.5375</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>45537.77083333333</v>
       </c>
       <c r="C71" s="2">
-        <v>45538.20625</v>
+        <v>45538.20208333334</v>
       </c>
       <c r="D71" s="2">
         <v>45538.538194444445</v>
@@ -1435,10 +1435,10 @@
         <v>45538.77083333333</v>
       </c>
       <c r="C72" s="2">
-        <v>45539.2</v>
+        <v>45539.20347222222</v>
       </c>
       <c r="D72" s="2">
-        <v>45539.52569444444</v>
+        <v>45539.53472222222</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1449,10 +1449,10 @@
         <v>45539.77083333333</v>
       </c>
       <c r="C73" s="2">
-        <v>45540.1875</v>
+        <v>45540.18958333333</v>
       </c>
       <c r="D73" s="2">
-        <v>45540.53194444445</v>
+        <v>45540.53402777778</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1463,10 +1463,10 @@
         <v>45540.77083333333</v>
       </c>
       <c r="C74" s="2">
-        <v>45541.21388888889</v>
+        <v>45541.20694444445</v>
       </c>
       <c r="D74" s="2">
-        <v>45541.53194444445</v>
+        <v>45541.524305555555</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1476,11 +1476,11 @@
       <c r="B75" s="1">
         <v>45541.77083333333</v>
       </c>
-      <c r="C75" s="2">
-        <v>45542.1875</v>
-      </c>
-      <c r="D75" s="2">
-        <v>45542.35416666667</v>
+      <c r="C75" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -1490,11 +1490,11 @@
       <c r="B76" s="1">
         <v>45543.77083333333</v>
       </c>
-      <c r="C76" s="2">
-        <v>45544.21736111111</v>
-      </c>
-      <c r="D76" s="2">
-        <v>45544.523611111115</v>
+      <c r="C76" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,7 +1505,7 @@
         <v>45544.77083333333</v>
       </c>
       <c r="C77" s="2">
-        <v>45545.20833333333</v>
+        <v>45545.19375</v>
       </c>
       <c r="D77" s="2">
         <v>45545.52916666667</v>
@@ -1513,114 +1513,114 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1">
         <v>45565.77083333333</v>
       </c>
       <c r="C78" s="2">
-        <v>45566.21736111111</v>
+        <v>45566.19583333333</v>
       </c>
       <c r="D78" s="2">
-        <v>45566.55</v>
+        <v>45566.52222222222</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1">
         <v>45566.77083333333</v>
       </c>
       <c r="C79" s="2">
-        <v>45567.214583333334</v>
+        <v>45567.211805555555</v>
       </c>
       <c r="D79" s="2">
-        <v>45567.544444444444</v>
+        <v>45567.506944444445</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1">
         <v>45567.77083333333</v>
       </c>
       <c r="C80" s="2">
-        <v>45568.20486111111</v>
+        <v>45568.21041666667</v>
       </c>
       <c r="D80" s="2">
-        <v>45568.52291666667</v>
+        <v>45568.54027777778</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1">
         <v>45568.77083333333</v>
       </c>
       <c r="C81" s="2">
-        <v>45569.19027777778</v>
+        <v>45569.19652777778</v>
       </c>
       <c r="D81" s="2">
-        <v>45569.54583333334</v>
+        <v>45569.538194444445</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1">
         <v>45569.77083333333</v>
       </c>
-      <c r="C82" s="2">
-        <v>45570.1875</v>
-      </c>
-      <c r="D82" s="2">
-        <v>45570.35416666667</v>
+      <c r="C82" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B83" s="1">
         <v>45571.77083333333</v>
       </c>
       <c r="C83" s="2">
-        <v>45572.19583333333</v>
+        <v>45572.19305555556</v>
       </c>
       <c r="D83" s="2">
-        <v>45572.549305555556</v>
+        <v>45572.52291666667</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B84" s="1">
         <v>45572.77083333333</v>
       </c>
       <c r="C84" s="2">
-        <v>45573.21597222222</v>
+        <v>45573.20625</v>
       </c>
       <c r="D84" s="2">
-        <v>45573.54652777778</v>
+        <v>45573.52291666667</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B85" s="1">
         <v>45573.77083333333</v>
       </c>
       <c r="C85" s="2">
-        <v>45574.21597222222</v>
+        <v>45574.20416666666</v>
       </c>
       <c r="D85" s="2">
-        <v>45574.56388888889</v>
+        <v>45574.527083333334</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -1631,10 +1631,10 @@
         <v>45596.77083333333</v>
       </c>
       <c r="C86" s="2">
-        <v>45597.21597222222</v>
+        <v>45597.21041666667</v>
       </c>
       <c r="D86" s="2">
-        <v>45597.527083333334</v>
+        <v>45597.566666666666</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -1644,11 +1644,11 @@
       <c r="B87" s="1">
         <v>45597.77083333333</v>
       </c>
-      <c r="C87" s="2">
-        <v>45598.1875</v>
-      </c>
-      <c r="D87" s="2">
-        <v>45598.35416666667</v>
+      <c r="C87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -1659,10 +1659,10 @@
         <v>45599.77083333333</v>
       </c>
       <c r="C88" s="2">
-        <v>45600.19930555555</v>
+        <v>45600.18958333333</v>
       </c>
       <c r="D88" s="2">
-        <v>45600.54375</v>
+        <v>45600.55</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -1673,10 +1673,10 @@
         <v>45600.77083333333</v>
       </c>
       <c r="C89" s="2">
-        <v>45601.211805555555</v>
+        <v>45601.20138888889</v>
       </c>
       <c r="D89" s="2">
-        <v>45601.50277777778</v>
+        <v>45601.53472222222</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,10 +1687,10 @@
         <v>45601.77083333333</v>
       </c>
       <c r="C90" s="2">
-        <v>45602.19861111111</v>
+        <v>45602.20347222222</v>
       </c>
       <c r="D90" s="2">
-        <v>45602.53472222222</v>
+        <v>45602.527083333334</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -1701,10 +1701,10 @@
         <v>45602.77083333333</v>
       </c>
       <c r="C91" s="2">
-        <v>45603.21736111111</v>
+        <v>45603.21597222222</v>
       </c>
       <c r="D91" s="2">
-        <v>45603.52083333333</v>
+        <v>45603.52986111111</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -1715,10 +1715,10 @@
         <v>45603.77083333333</v>
       </c>
       <c r="C92" s="2">
-        <v>45604.19097222222</v>
+        <v>45604.18819444445</v>
       </c>
       <c r="D92" s="2">
-        <v>45604.540972222225</v>
+        <v>45604.53680555556</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -1729,85 +1729,85 @@
         <v>45604.77083333333</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B94" s="1">
         <v>45627.77083333333</v>
       </c>
       <c r="C94" s="2">
-        <v>45628.20277777778</v>
+        <v>45628.2125</v>
       </c>
       <c r="D94" s="2">
-        <v>45628.52777777778</v>
+        <v>45628.53263888889</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B95" s="1">
         <v>45628.77083333333</v>
       </c>
       <c r="C95" s="2">
-        <v>45629.205555555556</v>
+        <v>45629.209027777775</v>
       </c>
       <c r="D95" s="2">
-        <v>45629.52986111111</v>
+        <v>45629.523611111115</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B96" s="1">
         <v>45629.77083333333</v>
       </c>
       <c r="C96" s="2">
-        <v>45630.211111111115</v>
+        <v>45630.194444444445</v>
       </c>
       <c r="D96" s="2">
-        <v>45630.50833333333</v>
+        <v>45630.5375</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B97" s="1">
         <v>45630.77083333333</v>
       </c>
       <c r="C97" s="2">
-        <v>45631.19791666667</v>
+        <v>45631.19930555555</v>
       </c>
       <c r="D97" s="2">
-        <v>45631.53611111111</v>
+        <v>45631.52986111111</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B98" s="1">
         <v>45631.77083333333</v>
       </c>
       <c r="C98" s="2">
-        <v>45632.19652777778</v>
+        <v>45632.2125</v>
       </c>
       <c r="D98" s="2">
-        <v>45632.52222222222</v>
+        <v>45632.54305555555</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B99" s="1">
         <v>45632.77083333333</v>
@@ -1821,30 +1821,30 @@
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B100" s="1">
         <v>45634.77083333333</v>
       </c>
       <c r="C100" s="2">
-        <v>45635.211111111115</v>
+        <v>45635.21805555555</v>
       </c>
       <c r="D100" s="2">
-        <v>45635.52569444444</v>
+        <v>45635.527083333334</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B101" s="1">
         <v>45635.77083333333</v>
       </c>
       <c r="C101" s="2">
-        <v>45636.20416666666</v>
+        <v>45636.20347222222</v>
       </c>
       <c r="D101" s="2">
-        <v>45636.5625</v>
+        <v>45636.53402777778</v>
       </c>
     </row>
   </sheetData>

</xml_diff>